<commit_message>
Reformulation of the model after discussion with Ruud
</commit_message>
<xml_diff>
--- a/Data/OneScenario/BaseCaseOld.xlsx
+++ b/Data/OneScenario/BaseCaseOld.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berendmarkhorst/Library/Mobile Documents/com~apple~CloudDocs/PhD/READINESS/08 - Trondheim/Data/OneScenario/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC25B551-4078-2241-9D5E-C8D0B9E138F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B08C99-84F0-E542-9CF4-605B708AEA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="24000" firstSheet="1" activeTab="14" xr2:uid="{D82E7092-1A4C-0041-9612-C431AA3B912B}"/>
+    <workbookView xWindow="-28800" yWindow="11300" windowWidth="28800" windowHeight="17500" firstSheet="5" activeTab="8" xr2:uid="{D82E7092-1A4C-0041-9612-C431AA3B912B}"/>
   </bookViews>
   <sheets>
     <sheet name="Visualisation" sheetId="7" r:id="rId1"/>
@@ -1608,15 +1608,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1627,6 +1618,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6452,7 +6452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71B95C95-5100-B242-B62A-0A2629824349}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -20483,6 +20483,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AH1:AW1"/>
+    <mergeCell ref="AH2:AW2"/>
+    <mergeCell ref="AH3:AO3"/>
+    <mergeCell ref="AP3:AW3"/>
+    <mergeCell ref="AX1:BM1"/>
+    <mergeCell ref="AX2:BM2"/>
+    <mergeCell ref="AX3:BE3"/>
+    <mergeCell ref="BF3:BM3"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="J3:Q3"/>
     <mergeCell ref="B1:Q1"/>
@@ -20491,14 +20499,6 @@
     <mergeCell ref="R2:AG2"/>
     <mergeCell ref="R3:Y3"/>
     <mergeCell ref="Z3:AG3"/>
-    <mergeCell ref="AH1:AW1"/>
-    <mergeCell ref="AH2:AW2"/>
-    <mergeCell ref="AH3:AO3"/>
-    <mergeCell ref="AP3:AW3"/>
-    <mergeCell ref="AX1:BM1"/>
-    <mergeCell ref="AX2:BM2"/>
-    <mergeCell ref="AX3:BE3"/>
-    <mergeCell ref="BF3:BM3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -21141,294 +21141,294 @@
       <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="64">
+      <c r="B3" s="61">
         <v>9</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
-      <c r="O3" s="65"/>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="66"/>
-      <c r="R3" s="64">
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="62"/>
+      <c r="O3" s="62"/>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="63"/>
+      <c r="R3" s="61">
         <v>9</v>
       </c>
-      <c r="S3" s="65"/>
-      <c r="T3" s="65"/>
-      <c r="U3" s="65"/>
-      <c r="V3" s="65"/>
-      <c r="W3" s="65"/>
-      <c r="X3" s="65"/>
-      <c r="Y3" s="65"/>
-      <c r="Z3" s="65"/>
-      <c r="AA3" s="65"/>
-      <c r="AB3" s="65"/>
-      <c r="AC3" s="65"/>
-      <c r="AD3" s="65"/>
-      <c r="AE3" s="65"/>
-      <c r="AF3" s="65"/>
-      <c r="AG3" s="66"/>
-      <c r="AH3" s="64">
+      <c r="S3" s="62"/>
+      <c r="T3" s="62"/>
+      <c r="U3" s="62"/>
+      <c r="V3" s="62"/>
+      <c r="W3" s="62"/>
+      <c r="X3" s="62"/>
+      <c r="Y3" s="62"/>
+      <c r="Z3" s="62"/>
+      <c r="AA3" s="62"/>
+      <c r="AB3" s="62"/>
+      <c r="AC3" s="62"/>
+      <c r="AD3" s="62"/>
+      <c r="AE3" s="62"/>
+      <c r="AF3" s="62"/>
+      <c r="AG3" s="63"/>
+      <c r="AH3" s="61">
         <v>9</v>
       </c>
-      <c r="AI3" s="65"/>
-      <c r="AJ3" s="65"/>
-      <c r="AK3" s="65"/>
-      <c r="AL3" s="65"/>
-      <c r="AM3" s="65"/>
-      <c r="AN3" s="65"/>
-      <c r="AO3" s="65"/>
-      <c r="AP3" s="65"/>
-      <c r="AQ3" s="65"/>
-      <c r="AR3" s="65"/>
-      <c r="AS3" s="65"/>
-      <c r="AT3" s="65"/>
-      <c r="AU3" s="65"/>
-      <c r="AV3" s="65"/>
-      <c r="AW3" s="66"/>
-      <c r="AX3" s="64">
+      <c r="AI3" s="62"/>
+      <c r="AJ3" s="62"/>
+      <c r="AK3" s="62"/>
+      <c r="AL3" s="62"/>
+      <c r="AM3" s="62"/>
+      <c r="AN3" s="62"/>
+      <c r="AO3" s="62"/>
+      <c r="AP3" s="62"/>
+      <c r="AQ3" s="62"/>
+      <c r="AR3" s="62"/>
+      <c r="AS3" s="62"/>
+      <c r="AT3" s="62"/>
+      <c r="AU3" s="62"/>
+      <c r="AV3" s="62"/>
+      <c r="AW3" s="63"/>
+      <c r="AX3" s="61">
         <v>9</v>
       </c>
-      <c r="AY3" s="65"/>
-      <c r="AZ3" s="65"/>
-      <c r="BA3" s="65"/>
-      <c r="BB3" s="65"/>
-      <c r="BC3" s="65"/>
-      <c r="BD3" s="65"/>
-      <c r="BE3" s="65"/>
-      <c r="BF3" s="65"/>
-      <c r="BG3" s="65"/>
-      <c r="BH3" s="65"/>
-      <c r="BI3" s="65"/>
-      <c r="BJ3" s="65"/>
-      <c r="BK3" s="65"/>
-      <c r="BL3" s="65"/>
-      <c r="BM3" s="66"/>
-      <c r="BN3" s="64">
+      <c r="AY3" s="62"/>
+      <c r="AZ3" s="62"/>
+      <c r="BA3" s="62"/>
+      <c r="BB3" s="62"/>
+      <c r="BC3" s="62"/>
+      <c r="BD3" s="62"/>
+      <c r="BE3" s="62"/>
+      <c r="BF3" s="62"/>
+      <c r="BG3" s="62"/>
+      <c r="BH3" s="62"/>
+      <c r="BI3" s="62"/>
+      <c r="BJ3" s="62"/>
+      <c r="BK3" s="62"/>
+      <c r="BL3" s="62"/>
+      <c r="BM3" s="63"/>
+      <c r="BN3" s="61">
         <v>17</v>
       </c>
-      <c r="BO3" s="65"/>
-      <c r="BP3" s="65"/>
-      <c r="BQ3" s="65"/>
-      <c r="BR3" s="65"/>
-      <c r="BS3" s="65"/>
-      <c r="BT3" s="65"/>
-      <c r="BU3" s="65"/>
-      <c r="BV3" s="65"/>
-      <c r="BW3" s="65"/>
-      <c r="BX3" s="65"/>
-      <c r="BY3" s="65"/>
-      <c r="BZ3" s="65"/>
-      <c r="CA3" s="65"/>
-      <c r="CB3" s="65"/>
-      <c r="CC3" s="66"/>
-      <c r="CD3" s="64">
+      <c r="BO3" s="62"/>
+      <c r="BP3" s="62"/>
+      <c r="BQ3" s="62"/>
+      <c r="BR3" s="62"/>
+      <c r="BS3" s="62"/>
+      <c r="BT3" s="62"/>
+      <c r="BU3" s="62"/>
+      <c r="BV3" s="62"/>
+      <c r="BW3" s="62"/>
+      <c r="BX3" s="62"/>
+      <c r="BY3" s="62"/>
+      <c r="BZ3" s="62"/>
+      <c r="CA3" s="62"/>
+      <c r="CB3" s="62"/>
+      <c r="CC3" s="63"/>
+      <c r="CD3" s="61">
         <v>17</v>
       </c>
-      <c r="CE3" s="65"/>
-      <c r="CF3" s="65"/>
-      <c r="CG3" s="65"/>
-      <c r="CH3" s="65"/>
-      <c r="CI3" s="65"/>
-      <c r="CJ3" s="65"/>
-      <c r="CK3" s="65"/>
-      <c r="CL3" s="65"/>
-      <c r="CM3" s="65"/>
-      <c r="CN3" s="65"/>
-      <c r="CO3" s="65"/>
-      <c r="CP3" s="65"/>
-      <c r="CQ3" s="65"/>
-      <c r="CR3" s="65"/>
-      <c r="CS3" s="66"/>
-      <c r="CT3" s="64">
+      <c r="CE3" s="62"/>
+      <c r="CF3" s="62"/>
+      <c r="CG3" s="62"/>
+      <c r="CH3" s="62"/>
+      <c r="CI3" s="62"/>
+      <c r="CJ3" s="62"/>
+      <c r="CK3" s="62"/>
+      <c r="CL3" s="62"/>
+      <c r="CM3" s="62"/>
+      <c r="CN3" s="62"/>
+      <c r="CO3" s="62"/>
+      <c r="CP3" s="62"/>
+      <c r="CQ3" s="62"/>
+      <c r="CR3" s="62"/>
+      <c r="CS3" s="63"/>
+      <c r="CT3" s="61">
         <v>17</v>
       </c>
-      <c r="CU3" s="65"/>
-      <c r="CV3" s="65"/>
-      <c r="CW3" s="65"/>
-      <c r="CX3" s="65"/>
-      <c r="CY3" s="65"/>
-      <c r="CZ3" s="65"/>
-      <c r="DA3" s="65"/>
-      <c r="DB3" s="65"/>
-      <c r="DC3" s="65"/>
-      <c r="DD3" s="65"/>
-      <c r="DE3" s="65"/>
-      <c r="DF3" s="65"/>
-      <c r="DG3" s="65"/>
-      <c r="DH3" s="65"/>
-      <c r="DI3" s="66"/>
-      <c r="DJ3" s="64">
+      <c r="CU3" s="62"/>
+      <c r="CV3" s="62"/>
+      <c r="CW3" s="62"/>
+      <c r="CX3" s="62"/>
+      <c r="CY3" s="62"/>
+      <c r="CZ3" s="62"/>
+      <c r="DA3" s="62"/>
+      <c r="DB3" s="62"/>
+      <c r="DC3" s="62"/>
+      <c r="DD3" s="62"/>
+      <c r="DE3" s="62"/>
+      <c r="DF3" s="62"/>
+      <c r="DG3" s="62"/>
+      <c r="DH3" s="62"/>
+      <c r="DI3" s="63"/>
+      <c r="DJ3" s="61">
         <v>17</v>
       </c>
-      <c r="DK3" s="65"/>
-      <c r="DL3" s="65"/>
-      <c r="DM3" s="65"/>
-      <c r="DN3" s="65"/>
-      <c r="DO3" s="65"/>
-      <c r="DP3" s="65"/>
-      <c r="DQ3" s="65"/>
-      <c r="DR3" s="65"/>
-      <c r="DS3" s="65"/>
-      <c r="DT3" s="65"/>
-      <c r="DU3" s="65"/>
-      <c r="DV3" s="65"/>
-      <c r="DW3" s="65"/>
-      <c r="DX3" s="65"/>
-      <c r="DY3" s="66"/>
-      <c r="DZ3" s="67">
+      <c r="DK3" s="62"/>
+      <c r="DL3" s="62"/>
+      <c r="DM3" s="62"/>
+      <c r="DN3" s="62"/>
+      <c r="DO3" s="62"/>
+      <c r="DP3" s="62"/>
+      <c r="DQ3" s="62"/>
+      <c r="DR3" s="62"/>
+      <c r="DS3" s="62"/>
+      <c r="DT3" s="62"/>
+      <c r="DU3" s="62"/>
+      <c r="DV3" s="62"/>
+      <c r="DW3" s="62"/>
+      <c r="DX3" s="62"/>
+      <c r="DY3" s="63"/>
+      <c r="DZ3" s="64">
         <v>25</v>
       </c>
-      <c r="EA3" s="62"/>
-      <c r="EB3" s="62"/>
-      <c r="EC3" s="62"/>
-      <c r="ED3" s="62"/>
-      <c r="EE3" s="62"/>
-      <c r="EF3" s="62"/>
-      <c r="EG3" s="62"/>
-      <c r="EH3" s="62"/>
-      <c r="EI3" s="62"/>
-      <c r="EJ3" s="62"/>
-      <c r="EK3" s="62"/>
-      <c r="EL3" s="62"/>
-      <c r="EM3" s="62"/>
-      <c r="EN3" s="62"/>
-      <c r="EO3" s="63"/>
-      <c r="EP3" s="61">
+      <c r="EA3" s="65"/>
+      <c r="EB3" s="65"/>
+      <c r="EC3" s="65"/>
+      <c r="ED3" s="65"/>
+      <c r="EE3" s="65"/>
+      <c r="EF3" s="65"/>
+      <c r="EG3" s="65"/>
+      <c r="EH3" s="65"/>
+      <c r="EI3" s="65"/>
+      <c r="EJ3" s="65"/>
+      <c r="EK3" s="65"/>
+      <c r="EL3" s="65"/>
+      <c r="EM3" s="65"/>
+      <c r="EN3" s="65"/>
+      <c r="EO3" s="66"/>
+      <c r="EP3" s="67">
         <v>25</v>
       </c>
-      <c r="EQ3" s="62"/>
-      <c r="ER3" s="62"/>
-      <c r="ES3" s="62"/>
-      <c r="ET3" s="62"/>
-      <c r="EU3" s="62"/>
-      <c r="EV3" s="62"/>
-      <c r="EW3" s="62"/>
-      <c r="EX3" s="62"/>
-      <c r="EY3" s="62"/>
-      <c r="EZ3" s="62"/>
-      <c r="FA3" s="62"/>
-      <c r="FB3" s="62"/>
-      <c r="FC3" s="62"/>
-      <c r="FD3" s="62"/>
-      <c r="FE3" s="63"/>
-      <c r="FF3" s="61">
+      <c r="EQ3" s="65"/>
+      <c r="ER3" s="65"/>
+      <c r="ES3" s="65"/>
+      <c r="ET3" s="65"/>
+      <c r="EU3" s="65"/>
+      <c r="EV3" s="65"/>
+      <c r="EW3" s="65"/>
+      <c r="EX3" s="65"/>
+      <c r="EY3" s="65"/>
+      <c r="EZ3" s="65"/>
+      <c r="FA3" s="65"/>
+      <c r="FB3" s="65"/>
+      <c r="FC3" s="65"/>
+      <c r="FD3" s="65"/>
+      <c r="FE3" s="66"/>
+      <c r="FF3" s="67">
         <v>25</v>
       </c>
-      <c r="FG3" s="62"/>
-      <c r="FH3" s="62"/>
-      <c r="FI3" s="62"/>
-      <c r="FJ3" s="62"/>
-      <c r="FK3" s="62"/>
-      <c r="FL3" s="62"/>
-      <c r="FM3" s="62"/>
-      <c r="FN3" s="62"/>
-      <c r="FO3" s="62"/>
-      <c r="FP3" s="62"/>
-      <c r="FQ3" s="62"/>
-      <c r="FR3" s="62"/>
-      <c r="FS3" s="62"/>
-      <c r="FT3" s="62"/>
-      <c r="FU3" s="63"/>
-      <c r="FV3" s="61">
+      <c r="FG3" s="65"/>
+      <c r="FH3" s="65"/>
+      <c r="FI3" s="65"/>
+      <c r="FJ3" s="65"/>
+      <c r="FK3" s="65"/>
+      <c r="FL3" s="65"/>
+      <c r="FM3" s="65"/>
+      <c r="FN3" s="65"/>
+      <c r="FO3" s="65"/>
+      <c r="FP3" s="65"/>
+      <c r="FQ3" s="65"/>
+      <c r="FR3" s="65"/>
+      <c r="FS3" s="65"/>
+      <c r="FT3" s="65"/>
+      <c r="FU3" s="66"/>
+      <c r="FV3" s="67">
         <v>25</v>
       </c>
-      <c r="FW3" s="62"/>
-      <c r="FX3" s="62"/>
-      <c r="FY3" s="62"/>
-      <c r="FZ3" s="62"/>
-      <c r="GA3" s="62"/>
-      <c r="GB3" s="62"/>
-      <c r="GC3" s="62"/>
-      <c r="GD3" s="62"/>
-      <c r="GE3" s="62"/>
-      <c r="GF3" s="62"/>
-      <c r="GG3" s="62"/>
-      <c r="GH3" s="62"/>
-      <c r="GI3" s="62"/>
-      <c r="GJ3" s="62"/>
-      <c r="GK3" s="63"/>
-      <c r="GL3" s="61">
+      <c r="FW3" s="65"/>
+      <c r="FX3" s="65"/>
+      <c r="FY3" s="65"/>
+      <c r="FZ3" s="65"/>
+      <c r="GA3" s="65"/>
+      <c r="GB3" s="65"/>
+      <c r="GC3" s="65"/>
+      <c r="GD3" s="65"/>
+      <c r="GE3" s="65"/>
+      <c r="GF3" s="65"/>
+      <c r="GG3" s="65"/>
+      <c r="GH3" s="65"/>
+      <c r="GI3" s="65"/>
+      <c r="GJ3" s="65"/>
+      <c r="GK3" s="66"/>
+      <c r="GL3" s="67">
         <v>33</v>
       </c>
-      <c r="GM3" s="62"/>
-      <c r="GN3" s="62"/>
-      <c r="GO3" s="62"/>
-      <c r="GP3" s="62"/>
-      <c r="GQ3" s="62"/>
-      <c r="GR3" s="62"/>
-      <c r="GS3" s="62"/>
-      <c r="GT3" s="62"/>
-      <c r="GU3" s="62"/>
-      <c r="GV3" s="62"/>
-      <c r="GW3" s="62"/>
-      <c r="GX3" s="62"/>
-      <c r="GY3" s="62"/>
-      <c r="GZ3" s="62"/>
-      <c r="HA3" s="63"/>
-      <c r="HB3" s="61">
+      <c r="GM3" s="65"/>
+      <c r="GN3" s="65"/>
+      <c r="GO3" s="65"/>
+      <c r="GP3" s="65"/>
+      <c r="GQ3" s="65"/>
+      <c r="GR3" s="65"/>
+      <c r="GS3" s="65"/>
+      <c r="GT3" s="65"/>
+      <c r="GU3" s="65"/>
+      <c r="GV3" s="65"/>
+      <c r="GW3" s="65"/>
+      <c r="GX3" s="65"/>
+      <c r="GY3" s="65"/>
+      <c r="GZ3" s="65"/>
+      <c r="HA3" s="66"/>
+      <c r="HB3" s="67">
         <v>33</v>
       </c>
-      <c r="HC3" s="62"/>
-      <c r="HD3" s="62"/>
-      <c r="HE3" s="62"/>
-      <c r="HF3" s="62"/>
-      <c r="HG3" s="62"/>
-      <c r="HH3" s="62"/>
-      <c r="HI3" s="62"/>
-      <c r="HJ3" s="62"/>
-      <c r="HK3" s="62"/>
-      <c r="HL3" s="62"/>
-      <c r="HM3" s="62"/>
-      <c r="HN3" s="62"/>
-      <c r="HO3" s="62"/>
-      <c r="HP3" s="62"/>
-      <c r="HQ3" s="63"/>
-      <c r="HR3" s="61">
+      <c r="HC3" s="65"/>
+      <c r="HD3" s="65"/>
+      <c r="HE3" s="65"/>
+      <c r="HF3" s="65"/>
+      <c r="HG3" s="65"/>
+      <c r="HH3" s="65"/>
+      <c r="HI3" s="65"/>
+      <c r="HJ3" s="65"/>
+      <c r="HK3" s="65"/>
+      <c r="HL3" s="65"/>
+      <c r="HM3" s="65"/>
+      <c r="HN3" s="65"/>
+      <c r="HO3" s="65"/>
+      <c r="HP3" s="65"/>
+      <c r="HQ3" s="66"/>
+      <c r="HR3" s="67">
         <v>33</v>
       </c>
-      <c r="HS3" s="62"/>
-      <c r="HT3" s="62"/>
-      <c r="HU3" s="62"/>
-      <c r="HV3" s="62"/>
-      <c r="HW3" s="62"/>
-      <c r="HX3" s="62"/>
-      <c r="HY3" s="62"/>
-      <c r="HZ3" s="62"/>
-      <c r="IA3" s="62"/>
-      <c r="IB3" s="62"/>
-      <c r="IC3" s="62"/>
-      <c r="ID3" s="62"/>
-      <c r="IE3" s="62"/>
-      <c r="IF3" s="62"/>
-      <c r="IG3" s="63"/>
-      <c r="IH3" s="61">
+      <c r="HS3" s="65"/>
+      <c r="HT3" s="65"/>
+      <c r="HU3" s="65"/>
+      <c r="HV3" s="65"/>
+      <c r="HW3" s="65"/>
+      <c r="HX3" s="65"/>
+      <c r="HY3" s="65"/>
+      <c r="HZ3" s="65"/>
+      <c r="IA3" s="65"/>
+      <c r="IB3" s="65"/>
+      <c r="IC3" s="65"/>
+      <c r="ID3" s="65"/>
+      <c r="IE3" s="65"/>
+      <c r="IF3" s="65"/>
+      <c r="IG3" s="66"/>
+      <c r="IH3" s="67">
         <v>33</v>
       </c>
-      <c r="II3" s="62"/>
-      <c r="IJ3" s="62"/>
-      <c r="IK3" s="62"/>
-      <c r="IL3" s="62"/>
-      <c r="IM3" s="62"/>
-      <c r="IN3" s="62"/>
-      <c r="IO3" s="62"/>
-      <c r="IP3" s="62"/>
-      <c r="IQ3" s="62"/>
-      <c r="IR3" s="62"/>
-      <c r="IS3" s="62"/>
-      <c r="IT3" s="62"/>
-      <c r="IU3" s="62"/>
-      <c r="IV3" s="62"/>
-      <c r="IW3" s="63"/>
+      <c r="II3" s="65"/>
+      <c r="IJ3" s="65"/>
+      <c r="IK3" s="65"/>
+      <c r="IL3" s="65"/>
+      <c r="IM3" s="65"/>
+      <c r="IN3" s="65"/>
+      <c r="IO3" s="65"/>
+      <c r="IP3" s="65"/>
+      <c r="IQ3" s="65"/>
+      <c r="IR3" s="65"/>
+      <c r="IS3" s="65"/>
+      <c r="IT3" s="65"/>
+      <c r="IU3" s="65"/>
+      <c r="IV3" s="65"/>
+      <c r="IW3" s="66"/>
     </row>
     <row r="4" spans="1:257" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
@@ -33665,41 +33665,35 @@
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="B1:Q1"/>
-    <mergeCell ref="R1:AG1"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="R2:AG2"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="J4:Q4"/>
-    <mergeCell ref="R4:Y4"/>
-    <mergeCell ref="Z4:AG4"/>
-    <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="R3:AG3"/>
-    <mergeCell ref="AH4:AO4"/>
-    <mergeCell ref="AP4:AW4"/>
-    <mergeCell ref="AX4:BE4"/>
-    <mergeCell ref="BF4:BM4"/>
-    <mergeCell ref="BN4:BU4"/>
-    <mergeCell ref="BV4:CC4"/>
-    <mergeCell ref="CD4:CK4"/>
-    <mergeCell ref="CL4:CS4"/>
-    <mergeCell ref="CT4:DA4"/>
-    <mergeCell ref="DB4:DI4"/>
-    <mergeCell ref="DJ4:DQ4"/>
-    <mergeCell ref="DR4:DY4"/>
-    <mergeCell ref="DZ4:EG4"/>
-    <mergeCell ref="EH4:EO4"/>
-    <mergeCell ref="EP4:EW4"/>
-    <mergeCell ref="EX4:FE4"/>
-    <mergeCell ref="FF4:FM4"/>
-    <mergeCell ref="FN4:FU4"/>
-    <mergeCell ref="FV4:GC4"/>
-    <mergeCell ref="GD4:GK4"/>
-    <mergeCell ref="GL4:GS4"/>
-    <mergeCell ref="GT4:HA4"/>
-    <mergeCell ref="HB4:HI4"/>
-    <mergeCell ref="HJ4:HQ4"/>
-    <mergeCell ref="HR4:HY4"/>
+    <mergeCell ref="HB2:HQ2"/>
+    <mergeCell ref="HR2:IG2"/>
+    <mergeCell ref="IH2:IW2"/>
+    <mergeCell ref="DZ2:EO2"/>
+    <mergeCell ref="EP2:FE2"/>
+    <mergeCell ref="FF2:FU2"/>
+    <mergeCell ref="FV2:GK2"/>
+    <mergeCell ref="GL2:HA2"/>
+    <mergeCell ref="AX2:BM2"/>
+    <mergeCell ref="BN2:CC2"/>
+    <mergeCell ref="CD2:CS2"/>
+    <mergeCell ref="CT2:DI2"/>
+    <mergeCell ref="DJ2:DY2"/>
+    <mergeCell ref="IH3:IW3"/>
+    <mergeCell ref="AH1:AW1"/>
+    <mergeCell ref="AX1:BM1"/>
+    <mergeCell ref="BN1:CC1"/>
+    <mergeCell ref="CD1:CS1"/>
+    <mergeCell ref="CT1:DI1"/>
+    <mergeCell ref="DJ1:DY1"/>
+    <mergeCell ref="DZ1:EO1"/>
+    <mergeCell ref="EP1:FE1"/>
+    <mergeCell ref="FF1:FU1"/>
+    <mergeCell ref="FV1:GK1"/>
+    <mergeCell ref="GL1:HA1"/>
+    <mergeCell ref="HB1:HQ1"/>
+    <mergeCell ref="HR1:IG1"/>
+    <mergeCell ref="IH1:IW1"/>
+    <mergeCell ref="AH2:AW2"/>
     <mergeCell ref="HZ4:IG4"/>
     <mergeCell ref="IH4:IO4"/>
     <mergeCell ref="IP4:IW4"/>
@@ -33716,35 +33710,41 @@
     <mergeCell ref="GL3:HA3"/>
     <mergeCell ref="HB3:HQ3"/>
     <mergeCell ref="HR3:IG3"/>
-    <mergeCell ref="IH3:IW3"/>
-    <mergeCell ref="AH1:AW1"/>
-    <mergeCell ref="AX1:BM1"/>
-    <mergeCell ref="BN1:CC1"/>
-    <mergeCell ref="CD1:CS1"/>
-    <mergeCell ref="CT1:DI1"/>
-    <mergeCell ref="DJ1:DY1"/>
-    <mergeCell ref="DZ1:EO1"/>
-    <mergeCell ref="EP1:FE1"/>
-    <mergeCell ref="FF1:FU1"/>
-    <mergeCell ref="FV1:GK1"/>
-    <mergeCell ref="GL1:HA1"/>
-    <mergeCell ref="HB1:HQ1"/>
-    <mergeCell ref="HR1:IG1"/>
-    <mergeCell ref="IH1:IW1"/>
-    <mergeCell ref="AH2:AW2"/>
-    <mergeCell ref="AX2:BM2"/>
-    <mergeCell ref="BN2:CC2"/>
-    <mergeCell ref="CD2:CS2"/>
-    <mergeCell ref="CT2:DI2"/>
-    <mergeCell ref="DJ2:DY2"/>
-    <mergeCell ref="HB2:HQ2"/>
-    <mergeCell ref="HR2:IG2"/>
-    <mergeCell ref="IH2:IW2"/>
-    <mergeCell ref="DZ2:EO2"/>
-    <mergeCell ref="EP2:FE2"/>
-    <mergeCell ref="FF2:FU2"/>
-    <mergeCell ref="FV2:GK2"/>
-    <mergeCell ref="GL2:HA2"/>
+    <mergeCell ref="GL4:GS4"/>
+    <mergeCell ref="GT4:HA4"/>
+    <mergeCell ref="HB4:HI4"/>
+    <mergeCell ref="HJ4:HQ4"/>
+    <mergeCell ref="HR4:HY4"/>
+    <mergeCell ref="EX4:FE4"/>
+    <mergeCell ref="FF4:FM4"/>
+    <mergeCell ref="FN4:FU4"/>
+    <mergeCell ref="FV4:GC4"/>
+    <mergeCell ref="GD4:GK4"/>
+    <mergeCell ref="DJ4:DQ4"/>
+    <mergeCell ref="DR4:DY4"/>
+    <mergeCell ref="DZ4:EG4"/>
+    <mergeCell ref="EH4:EO4"/>
+    <mergeCell ref="EP4:EW4"/>
+    <mergeCell ref="BV4:CC4"/>
+    <mergeCell ref="CD4:CK4"/>
+    <mergeCell ref="CL4:CS4"/>
+    <mergeCell ref="CT4:DA4"/>
+    <mergeCell ref="DB4:DI4"/>
+    <mergeCell ref="AH4:AO4"/>
+    <mergeCell ref="AP4:AW4"/>
+    <mergeCell ref="AX4:BE4"/>
+    <mergeCell ref="BF4:BM4"/>
+    <mergeCell ref="BN4:BU4"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="R1:AG1"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="R2:AG2"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="J4:Q4"/>
+    <mergeCell ref="R4:Y4"/>
+    <mergeCell ref="Z4:AG4"/>
+    <mergeCell ref="B3:Q3"/>
+    <mergeCell ref="R3:AG3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -34344,8 +34344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D89E28-915C-F54C-B37A-2FAB20B0DB56}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34454,7 +34454,7 @@
         <v>343</v>
       </c>
       <c r="B13">
-        <v>1.2</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -34462,7 +34462,7 @@
         <v>344</v>
       </c>
       <c r="B14">
-        <v>1.5</v>
+        <v>1.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>